<commit_message>
Done add export excel
</commit_message>
<xml_diff>
--- a/SMESData/Resources/Temp.xlsx
+++ b/SMESData/Resources/Temp.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="MQC" sheetId="3" r:id="rId1"/>
+    <sheet name="managers" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -27,10 +28,13 @@
     <t>Date</t>
   </si>
   <si>
+    <t>{{Title}}</t>
+  </si>
+  <si>
     <t>Line</t>
   </si>
   <si>
-    <t>Out put</t>
+    <t>Out Put</t>
   </si>
   <si>
     <t>No Good</t>
@@ -42,10 +46,7 @@
     <t>Daily Target</t>
   </si>
   <si>
-    <t>NG rate (%)</t>
-  </si>
-  <si>
-    <t>{{Title}}</t>
+    <t>%NG</t>
   </si>
   <si>
     <t>{{MQC.Model}}</t>
@@ -76,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +92,13 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -158,10 +166,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,108 +486,80 @@
     <col min="4" max="4" width="2.44140625" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="17.44140625" customWidth="1"/>
     <col min="9" max="9" width="25.109375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="5.6640625" customWidth="1"/>
     <col min="13" max="13" width="2.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" customWidth="1"/>
-    <col min="17" max="17" width="5.5546875" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" customWidth="1"/>
+    <col min="17" max="17" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="5" spans="2:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5" s="3"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="2:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -593,4 +582,112 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.77734375" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="5" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update PQC Export Excel
</commit_message>
<xml_diff>
--- a/SMESData/Resources/Temp.xlsx
+++ b/SMESData/Resources/Temp.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="managers" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="MQC" sheetId="4" r:id="rId1"/>
+    <sheet name="PQC" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Model</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>{{Title}}</t>
-  </si>
-  <si>
     <t>Line</t>
   </si>
   <si>
@@ -71,6 +68,36 @@
   </si>
   <si>
     <t>{{MQC.NG_rate_realtime}}</t>
+  </si>
+  <si>
+    <t>{{PQC.Date}}</t>
+  </si>
+  <si>
+    <t>{{PQC.Line}}</t>
+  </si>
+  <si>
+    <t>{{PQC.OUTPUT}}</t>
+  </si>
+  <si>
+    <t>{{PQC.NOGOOD}}</t>
+  </si>
+  <si>
+    <t>{{PQC.Total}}</t>
+  </si>
+  <si>
+    <t>{{PQC.NG_rate_realtime}}</t>
+  </si>
+  <si>
+    <t>{{PQC.Model}}</t>
+  </si>
+  <si>
+    <t>{{Title1}}</t>
+  </si>
+  <si>
+    <t>{{Title2}}</t>
+  </si>
+  <si>
+    <t>{{PQC.Target}}</t>
   </si>
 </sst>
 </file>
@@ -113,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,41 +163,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -183,16 +181,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,112 +465,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q6"/>
+  <dimension ref="B1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" customWidth="1"/>
-    <col min="3" max="3" width="3.5546875" customWidth="1"/>
-    <col min="4" max="4" width="2.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
-    <col min="9" max="9" width="25.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" customWidth="1"/>
-    <col min="13" max="13" width="2.77734375" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" customWidth="1"/>
-    <col min="17" max="17" width="4.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="F1" s="8" t="s">
+    <row r="1" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="5" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="5" spans="2:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="2:17" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="F1:K3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -589,102 +578,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.77734375" customWidth="1"/>
     <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="5" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-    </row>
-    <row r="2" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="5" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="6" spans="2:10" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>